<commit_message>
transformacion y limpieza de datos (agrupar, eliminar valores nulos y convertir formatos)
</commit_message>
<xml_diff>
--- a/Data/Datos_transformados/museos_transformacion.xlsx
+++ b/Data/Datos_transformados/museos_transformacion.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5861A9A5-D0F1-4950-9A0A-52D798DEEFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368C21C5-24E9-4D38-B81A-F0B0F0D99BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-990" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Responses" sheetId="1" r:id="rId1"/>
+    <sheet name="datos_brutos" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -1160,7 +1161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1729"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
@@ -1173,11 +1174,12 @@
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="166.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="140.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
     <col min="14" max="14" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="23" bestFit="1" customWidth="1"/>
   </cols>
@@ -74289,4 +74291,16 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2DC34C-FDCB-4336-BE5C-12643E31528B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>